<commit_message>
add changes at report
</commit_message>
<xml_diff>
--- a/Отчет 31.08.2015.xlsx
+++ b/Отчет 31.08.2015.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7065" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7065" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Закупленно" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>№</t>
   </si>
@@ -126,6 +126,27 @@
   </si>
   <si>
     <t>Травка оснойной управляющей платы</t>
+  </si>
+  <si>
+    <t>DG308-2,54-03</t>
+  </si>
+  <si>
+    <t>pbs-40</t>
+  </si>
+  <si>
+    <t>pbs-20R</t>
+  </si>
+  <si>
+    <t>RC0805FR-071K1L</t>
+  </si>
+  <si>
+    <t>RES0805 10K</t>
+  </si>
+  <si>
+    <t>PLS-40</t>
+  </si>
+  <si>
+    <t>основная плата</t>
   </si>
 </sst>
 </file>
@@ -443,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -457,7 +478,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -508,69 +528,71 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -849,7 +871,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -860,7 +882,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -872,14 +894,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickTop="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="25"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
@@ -905,17 +927,18 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="2">
-        <v>21</v>
+        <v>21.07</v>
       </c>
       <c r="D3" s="2">
         <v>18.989999999999998</v>
       </c>
-      <c r="E3" s="2">
-        <v>400</v>
+      <c r="E3" s="48">
+        <f>C3*D3</f>
+        <v>400.11929999999995</v>
       </c>
       <c r="F3" s="5"/>
     </row>
@@ -923,61 +946,127 @@
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="5"/>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="2">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="E4" s="48">
+        <f t="shared" ref="E4:E19" si="0">C4*D4</f>
+        <v>173.27999999999997</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="5"/>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>8.32</v>
+      </c>
+      <c r="E5" s="48">
+        <f t="shared" si="0"/>
+        <v>8.32</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="5"/>
+      <c r="B6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>6.99</v>
+      </c>
+      <c r="E6" s="48">
+        <f t="shared" si="0"/>
+        <v>6.99</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="5"/>
+      <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>8.24</v>
+      </c>
+      <c r="E7" s="48">
+        <f t="shared" si="0"/>
+        <v>8.24</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="5"/>
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="E8" s="48">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="5"/>
+      <c r="B9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="E9" s="48">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="3">
@@ -986,7 +1075,10 @@
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6">
@@ -996,7 +1088,10 @@
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6">
@@ -1006,7 +1101,10 @@
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6">
@@ -1016,7 +1114,10 @@
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6">
@@ -1026,82 +1127,100 @@
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="E14" s="48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="17">
+      <c r="A15" s="16">
         <v>13</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="19"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="18"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="17">
+      <c r="A16" s="16">
         <v>14</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="19"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="18"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="17">
+      <c r="A17" s="16">
         <v>15</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="19"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="18"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="17">
+      <c r="A18" s="16">
         <v>16</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="19"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="18"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="17">
+      <c r="A19" s="16">
         <v>16</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="19"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="18"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="7">
-        <f>SUM(E5:E19,E3:E4)</f>
-        <v>400</v>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="49">
+        <f>SUM(E3:E19)</f>
+        <v>606.94929999999999</v>
       </c>
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="7">
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="49">
         <f>1410-E20</f>
-        <v>1010</v>
+        <v>803.05070000000001</v>
       </c>
       <c r="F21" s="6"/>
     </row>
@@ -1113,6 +1232,7 @@
     <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1120,7 +1240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
@@ -1133,41 +1253,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
       <c r="L2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1179,279 +1299,269 @@
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="8">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="31" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="32"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="21">
+      <c r="J3" s="30"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="20">
         <v>40</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="9">
         <v>42241</v>
       </c>
-      <c r="N3" s="21">
+      <c r="N3" s="20">
         <v>2.5</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30" t="s">
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="8">
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="7">
         <v>40</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="9">
         <v>42242</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30" t="s">
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="8">
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="7">
         <v>40</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="9">
         <v>42243</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="7">
         <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30" t="s">
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="8">
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="7">
         <v>40</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="9">
         <v>42244</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="8"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="7"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="9">
+      <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="9"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="8"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="9">
+      <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="20"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="19"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>8</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="13"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="12"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="13">
+      <c r="A11" s="12">
         <v>9</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="13"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="12"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="14">
+      <c r="A12" s="13">
         <v>10</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="14"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="13"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="14">
+      <c r="A13" s="13">
         <v>11</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="14"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="13"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="11">
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="10">
         <f>SUM(L3:L13)</f>
         <v>160</v>
       </c>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12">
+      <c r="M14" s="11"/>
+      <c r="N14" s="11">
         <f>SUM(N3:N13)</f>
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="I3:K3"/>
     <mergeCell ref="A14:K14"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="I2:K2"/>
@@ -1468,6 +1578,16 @@
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="B12:H12"/>
     <mergeCell ref="I12:K12"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="I3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1477,7 +1597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O12" sqref="O12:Q12"/>
     </sheetView>
   </sheetViews>
@@ -1487,202 +1607,202 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="40"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36" t="s">
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36" t="s">
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36" t="s">
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
     </row>
     <row r="3" spans="1:20" ht="31.5" customHeight="1">
-      <c r="A3" s="16">
+      <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="37">
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="33">
         <v>1</v>
       </c>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37">
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33">
         <v>2</v>
       </c>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37">
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33">
         <v>75</v>
       </c>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37">
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33">
         <f>(SUM(H3:N3)*O3)</f>
         <v>225</v>
       </c>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
     </row>
     <row r="4" spans="1:20" ht="31.5" customHeight="1">
-      <c r="A4" s="22">
+      <c r="A4" s="21">
         <v>2</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="43">
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="37">
         <v>1</v>
       </c>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="43">
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="37">
         <v>4</v>
       </c>
-      <c r="M4" s="44"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="43">
+      <c r="M4" s="38"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="37">
         <v>75</v>
       </c>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="37">
+      <c r="P4" s="38"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="33">
         <f>(SUM(H4:N4)*O4)</f>
         <v>375</v>
       </c>
-      <c r="S4" s="37"/>
-      <c r="T4" s="37"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
     </row>
     <row r="5" spans="1:20" ht="31.5" customHeight="1">
-      <c r="A5" s="22">
+      <c r="A5" s="21">
         <v>3</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="43">
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="37">
         <v>1</v>
       </c>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="43">
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="37">
         <v>2</v>
       </c>
-      <c r="M5" s="44"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="43">
+      <c r="M5" s="38"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="37">
         <v>75</v>
       </c>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="37">
+      <c r="P5" s="38"/>
+      <c r="Q5" s="39"/>
+      <c r="R5" s="33">
         <f>(SUM(H5:N5)*O5)</f>
         <v>225</v>
       </c>
-      <c r="S5" s="37"/>
-      <c r="T5" s="37"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33"/>
     </row>
     <row r="6" spans="1:20" ht="31.5" customHeight="1">
-      <c r="A6" s="22">
+      <c r="A6" s="21">
         <v>4</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="43">
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="37">
         <v>1</v>
       </c>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="43">
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="37">
         <v>4</v>
       </c>
-      <c r="M6" s="44"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="43">
+      <c r="M6" s="38"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="37">
         <v>75</v>
       </c>
-      <c r="P6" s="44"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="37">
+      <c r="P6" s="38"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="33">
         <f>(SUM(H6:N6)*O6)</f>
         <v>375</v>
       </c>
-      <c r="S6" s="37"/>
-      <c r="T6" s="37"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="33"/>
     </row>
     <row r="7" spans="1:20" ht="15" customHeight="1">
       <c r="A7" s="42" t="s">
@@ -1694,201 +1814,240 @@
       <c r="E7" s="42"/>
       <c r="F7" s="42"/>
       <c r="G7" s="42"/>
-      <c r="H7" s="38">
+      <c r="H7" s="40">
         <f>SUM(H3:K6)</f>
         <v>4</v>
       </c>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38">
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40">
         <f>SUM(L3:N6)</f>
         <v>12</v>
       </c>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="38">
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40">
         <v>75</v>
       </c>
-      <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="38">
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40">
         <f>SUM(R3:T6)</f>
         <v>1200</v>
       </c>
-      <c r="S7" s="38"/>
-      <c r="T7" s="38"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
     </row>
     <row r="8" spans="1:20" ht="15" customHeight="1">
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="34"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="47"/>
     </row>
     <row r="9" spans="1:20" ht="15" customHeight="1">
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="34"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="47"/>
+      <c r="P9" s="47"/>
+      <c r="Q9" s="47"/>
     </row>
     <row r="10" spans="1:20" ht="15" customHeight="1">
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="34"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="47"/>
     </row>
     <row r="11" spans="1:20" ht="15" customHeight="1">
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
-      <c r="P11" s="34"/>
-      <c r="Q11" s="34"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="47"/>
     </row>
     <row r="12" spans="1:20" ht="15" customHeight="1">
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="34"/>
-      <c r="P12" s="34"/>
-      <c r="Q12" s="34"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="47"/>
     </row>
     <row r="13" spans="1:20" ht="15" customHeight="1">
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="34"/>
-      <c r="Q13" s="34"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="47"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="47"/>
     </row>
     <row r="14" spans="1:20" ht="15" customHeight="1">
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="34"/>
-      <c r="P14" s="34"/>
-      <c r="Q14" s="34"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="47"/>
+      <c r="P14" s="47"/>
+      <c r="Q14" s="47"/>
     </row>
     <row r="15" spans="1:20" ht="15" customHeight="1">
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
-      <c r="P15" s="34"/>
-      <c r="Q15" s="34"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="47"/>
     </row>
     <row r="16" spans="1:20" ht="15" customHeight="1">
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="34"/>
-      <c r="P16" s="34"/>
-      <c r="Q16" s="34"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="O13:Q13"/>
+    <mergeCell ref="O14:Q14"/>
+    <mergeCell ref="O15:Q15"/>
+    <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="R3:T3"/>
     <mergeCell ref="R7:T7"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:K2"/>
@@ -1905,51 +2064,12 @@
     <mergeCell ref="H5:K5"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="L16:N16"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="O13:Q13"/>
-    <mergeCell ref="O14:Q14"/>
-    <mergeCell ref="O15:Q15"/>
-    <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="R6:T6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>